<commit_message>
created and applied API
</commit_message>
<xml_diff>
--- a/data/Synthetic_data.xlsx
+++ b/data/Synthetic_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thealanturininstitute-my.sharepoint.com/personal/dletch_turing_ac_uk/Documents/Documents/Data/Data- September/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thealanturininstitute-my.sharepoint.com/personal/dletch_turing_ac_uk/Documents/Documents/R Studio/DaisyProject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43818241-65B4-9A4C-9D64-4F7D628CA6DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{43818241-65B4-9A4C-9D64-4F7D628CA6DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{92071835-BEF6-9244-BB1F-8C2857F956E6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23240" windowHeight="12560" xr2:uid="{3A636213-70DF-EF40-9203-74C541530B51}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="12580" windowHeight="16020" xr2:uid="{3A636213-70DF-EF40-9203-74C541530B51}"/>
   </bookViews>
   <sheets>
     <sheet name="Master dummy data" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="Packed circle" sheetId="7" r:id="rId6"/>
     <sheet name="Collaboration plot" sheetId="8" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master dummy data'!$A$1:$O$80</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -778,7 +781,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -790,7 +793,7 @@
     <col min="5" max="5" width="6.1640625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="11" customWidth="1"/>
     <col min="9" max="9" width="5.1640625" style="9" customWidth="1"/>
     <col min="10" max="11" width="10.5" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="9" bestFit="1" customWidth="1"/>
@@ -4561,6 +4564,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O80" xr:uid="{76118F98-AA34-FD44-BA6B-BD8215BC9D58}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O80">
     <sortCondition ref="A2:A80"/>
   </sortState>
@@ -14338,8 +14342,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A5C6F44-D892-40F7-9E18-95AFC5A81A59}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4e515479-2dcd-4a7a-9f98-fabd656adaef"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3d6f0696-eb69-4a21-a5cb-887eceb94773"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>